<commit_message>
updated excel files data
</commit_message>
<xml_diff>
--- a/Test_Data/ExistingUserLoginDetails.xlsx
+++ b/Test_Data/ExistingUserLoginDetails.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anshul\PycharmProjects\Automation Scripts\Test_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{580576CE-8B71-4950-B60A-033A8E4C6358}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E05AFF07-64E5-471B-A8DF-123A691D3FBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3380" yWindow="3380" windowWidth="16920" windowHeight="10450" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,16 +33,16 @@
     <t>User Password</t>
   </si>
   <si>
-    <t>anshulgupta1791@gmail.com</t>
-  </si>
-  <si>
-    <t>Anshul</t>
-  </si>
-  <si>
     <t>Pass</t>
   </si>
   <si>
     <t>Expected Result</t>
+  </si>
+  <si>
+    <t>anshultest@test.com</t>
+  </si>
+  <si>
+    <t>AnshulTest</t>
   </si>
 </sst>
 </file>
@@ -374,7 +374,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -391,18 +391,18 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
         <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" t="s">
-        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>